<commit_message>
test: update test excel files to match global row rules
</commit_message>
<xml_diff>
--- a/ExternalTestData/Excel/LogicTest.xlsx
+++ b/ExternalTestData/Excel/LogicTest.xlsx
@@ -3,63 +3,68 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS Project\ExcelBinder\ExternalTestData\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016E1693-4D43-40FA-9E9D-C00B2101EA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6765" yWindow="4635" windowWidth="21600" windowHeight="11295"/>
+    <workbookView xWindow="1905" yWindow="2580" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BattleLogic" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReturnType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Formula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CalculateDamage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int atk, int def</t>
-  </si>
-  <si>
-    <t xml:space="preserve">atk - def &gt; 0 ? atk - def : 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GetExpNeeded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">long</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(long)Math.Pow(level, 3) * 100</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># Dummy Row (Ignored by ExcelBinder)</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ReturnType</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>CalculateDamage</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>int atk, int def</t>
+  </si>
+  <si>
+    <t>atk - def &gt; 0 ? atk - def : 1</t>
+  </si>
+  <si>
+    <t>GetExpNeeded</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>int level</t>
+  </si>
+  <si>
+    <t>(long)Math.Pow(level, 3) * 100</t>
+  </si>
+  <si>
+    <t># Dummy Row (Ignored by ExcelBinder)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -109,11 +114,11 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -407,7 +412,7 @@
   <a:objectDefaults>
     <a:lnDef>
       <a:spPr/>
-      <a:bodyPr rtlCol="0"/>
+      <a:bodyPr/>
       <a:lstStyle/>
       <a:style>
         <a:lnRef idx="2">
@@ -435,11 +440,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -450,50 +455,50 @@
     <col min="4" max="4" width="29.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="0" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="0" t="s">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="0" t="s">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>